<commit_message>
STRAV-15 correct some column datatypes
</commit_message>
<xml_diff>
--- a/Documentation/Strava DB data modelling.xlsx
+++ b/Documentation/Strava DB data modelling.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="599" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8ED7D1F-590A-43FE-9834-E57951D9A8C8}"/>
+  <xr:revisionPtr revIDLastSave="629" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516B215A-1413-4844-977C-2C3DC511D897}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API fields" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="184">
   <si>
     <t>SQL script generated via formula pt1</t>
   </si>
@@ -401,109 +401,118 @@
     <t>ID</t>
   </si>
   <si>
+    <t>UNIQUEIDENTIFIER</t>
+  </si>
+  <si>
+    <t>DEFAULT NEWID()</t>
+  </si>
+  <si>
+    <t>NVARCHAR(250)</t>
+  </si>
+  <si>
+    <t>athlete_id</t>
+  </si>
+  <si>
+    <t>athlete_resource_state</t>
+  </si>
+  <si>
+    <t>activity_type</t>
+  </si>
+  <si>
+    <t>activity_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> map_id</t>
+  </si>
+  <si>
+    <t>map_summary_polyline</t>
+  </si>
+  <si>
+    <t>NVARCHAR(MAX)</t>
+  </si>
+  <si>
+    <t>map_resource_state</t>
+  </si>
+  <si>
+    <t>date_created</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>DEFAULT GETDATE()</t>
+  </si>
+  <si>
+    <t>date_processed</t>
+  </si>
+  <si>
+    <t>DEFAULT NULL</t>
+  </si>
+  <si>
+    <t>processed_as</t>
+  </si>
+  <si>
+    <t>VARCHAR(250)</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>Staging.Activities</t>
+  </si>
+  <si>
+    <t>NOT NULL PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>NVARCHAR(50)</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>NUMERIC(10, 2)</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>NUMERIC(5, 1)</t>
+  </si>
+  <si>
+    <t>activity_type_id</t>
+  </si>
+  <si>
+    <t>NVARCHAR(100)</t>
+  </si>
+  <si>
+    <t>BIT NOT NULL</t>
+  </si>
+  <si>
+    <t>NUMERIC(3, 1)</t>
+  </si>
+  <si>
+    <t>NUMERIC(4, 1)</t>
+  </si>
+  <si>
+    <t>Reporting.FACT_activities</t>
+  </si>
+  <si>
+    <t>Reporting.DIM_activity_type</t>
+  </si>
+  <si>
+    <t>staging_id</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY REFERENCES Staging.Activities(ID)</t>
+  </si>
+  <si>
+    <t>Reporting.DIM_gear</t>
+  </si>
+  <si>
+    <t>NUMERIC(10, 1)</t>
+  </si>
+  <si>
     <t>UNIQUEIDENTIFER</t>
-  </si>
-  <si>
-    <t>DEFAULT NEWID()</t>
-  </si>
-  <si>
-    <t>NVARCHAR(250)</t>
-  </si>
-  <si>
-    <t>athlete_id</t>
-  </si>
-  <si>
-    <t>athlete_resource_state</t>
-  </si>
-  <si>
-    <t>activity_type</t>
-  </si>
-  <si>
-    <t>activity_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> map_id</t>
-  </si>
-  <si>
-    <t>map_summary_polyline</t>
-  </si>
-  <si>
-    <t>NVARCHAR(MAX)</t>
-  </si>
-  <si>
-    <t>map_resource_state</t>
-  </si>
-  <si>
-    <t>date_created</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>DEFAULT GETDATE()</t>
-  </si>
-  <si>
-    <t>date_processed</t>
-  </si>
-  <si>
-    <t>DEFAULT NULL</t>
-  </si>
-  <si>
-    <t>processed_as</t>
-  </si>
-  <si>
-    <t>VARCHAR(250)</t>
-  </si>
-  <si>
-    <t>);</t>
-  </si>
-  <si>
-    <t>Staging.Activities</t>
-  </si>
-  <si>
-    <t>NOT NULL PRIMARY KEY</t>
-  </si>
-  <si>
-    <t>INT</t>
-  </si>
-  <si>
-    <t>NOT NULL</t>
-  </si>
-  <si>
-    <t>NUMERIC(10, 2)</t>
-  </si>
-  <si>
-    <t>activity_type_id</t>
-  </si>
-  <si>
-    <t>NVARCHAR(50)</t>
-  </si>
-  <si>
-    <t>BOOLEAN</t>
-  </si>
-  <si>
-    <t>NUMERIC(2, 1)</t>
-  </si>
-  <si>
-    <t>NUMERIC(3, 1)</t>
-  </si>
-  <si>
-    <t>Reporting.FACT_activities</t>
-  </si>
-  <si>
-    <t>Reporting.DIM_activity_type</t>
-  </si>
-  <si>
-    <t>staging_id</t>
-  </si>
-  <si>
-    <t>FOREIGN KEY REFERENCES Staging.Activities(ID)</t>
-  </si>
-  <si>
-    <t>Reporting.DIM_gear</t>
-  </si>
-  <si>
-    <t>NUMERIC(10, 1)</t>
   </si>
   <si>
     <t>FOREIGN KEY REFERENCES Reporting.DIM_activity_type(activity_type_id)</t>
@@ -1874,7 +1883,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1920,7 +1929,7 @@
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT(A3, " ", B3,  " ", C3, ",")</f>
-        <v>ID UNIQUEIDENTIFER DEFAULT NEWID(),</v>
+        <v>ID UNIQUEIDENTIFIER DEFAULT NEWID(),</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2606,8 +2615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77B814F-9F70-4B91-9F92-4045C1E00E64}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2655,7 +2664,7 @@
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT(A3, " ", B3,  " ", C3, ",")</f>
-        <v>ID UNIQUEIDENTIFER NOT NULL PRIMARY KEY,</v>
+        <v>ID UNIQUEIDENTIFIER NOT NULL PRIMARY KEY,</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2670,7 +2679,7 @@
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(A4, " ", B4,  " ", C4, ",")</f>
-        <v>athlete_id INT NOT NULL,</v>
+        <v>athlete_id NVARCHAR(50) NOT NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2705,7 +2714,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D7" t="str">
         <f>_xlfn.CONCAT(A7, " ", B7,  " ", C7, ",")</f>
@@ -2717,7 +2726,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D8" t="str">
         <f>_xlfn.CONCAT(A8, " ", B8,  " ", C8, ",")</f>
@@ -2729,19 +2738,19 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D9" t="str">
         <f>_xlfn.CONCAT(A9, " ", B9,  " ", C9, ",")</f>
-        <v>total_elevation_gain INT ,</v>
+        <v>total_elevation_gain NUMERIC(5, 1) ,</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
         <v>147</v>
-      </c>
-      <c r="B10" t="s">
-        <v>144</v>
       </c>
       <c r="D10" t="str">
         <f>_xlfn.CONCAT(A10, " ", B10,  " ", C10, ",")</f>
@@ -2753,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D11" t="str">
         <f>_xlfn.CONCAT(A11, " ", B11,  " ", C11, ",")</f>
@@ -2772,7 +2781,7 @@
       </c>
       <c r="D12" t="str">
         <f>_xlfn.CONCAT(A12, " ", B12,  " ", C12, ",")</f>
-        <v>activity_id INT NOT NULL,</v>
+        <v>activity_id NVARCHAR(50) NOT NULL,</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2780,14 +2789,11 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.CONCAT(A13, " ", B13,  " ", C13, ",")</f>
-        <v>external_id NVARCHAR(50) NOT NULL,</v>
+        <v>external_id NVARCHAR(100) ,</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2810,7 +2816,7 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D15" t="str">
         <f>_xlfn.CONCAT(A15, " ", B15,  " ", C15, ",")</f>
@@ -2822,7 +2828,7 @@
         <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D16" t="str">
         <f>_xlfn.CONCAT(A16, " ", B16,  " ", C16, ",")</f>
@@ -2834,7 +2840,7 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D17" t="str">
         <f>_xlfn.CONCAT(A17, " ", B17,  " ", C17, ",")</f>
@@ -2846,7 +2852,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D18" t="str">
         <f>_xlfn.CONCAT(A18, " ", B18,  " ", C18, ",")</f>
@@ -2858,7 +2864,7 @@
         <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D19" t="str">
         <f>_xlfn.CONCAT(A19, " ", B19,  " ", C19, ",")</f>
@@ -2870,11 +2876,11 @@
         <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D20" t="str">
         <f>_xlfn.CONCAT(A20, " ", B20,  " ", C20, ",")</f>
-        <v>private BOOLEAN ,</v>
+        <v>private BIT NOT NULL ,</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2886,7 +2892,7 @@
       </c>
       <c r="D21" t="str">
         <f>_xlfn.CONCAT(A21, " ", B21,  " ", C21, ",")</f>
-        <v>gear_id INT ,</v>
+        <v>gear_id NVARCHAR(50) ,</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2894,11 +2900,11 @@
         <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D22" t="str">
         <f>_xlfn.CONCAT(A22, " ", B22,  " ", C22, ",")</f>
-        <v>average_speed NUMERIC(2, 1) ,</v>
+        <v>average_speed NUMERIC(3, 1) ,</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2906,11 +2912,11 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D23" t="str">
         <f>_xlfn.CONCAT(A23, " ", B23,  " ", C23, ",")</f>
-        <v>max_speed NUMERIC(2, 1) ,</v>
+        <v>max_speed NUMERIC(3, 1) ,</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2918,11 +2924,11 @@
         <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D24" t="str">
         <f>_xlfn.CONCAT(A24, " ", B24,  " ", C24, ",")</f>
-        <v>average_heartrate NUMERIC(3, 1) ,</v>
+        <v>average_heartrate NUMERIC(4, 1) ,</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2930,11 +2936,11 @@
         <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D25" t="str">
         <f>_xlfn.CONCAT(A25, " ", B25,  " ", C25, ",")</f>
-        <v>max_heartrate NUMERIC(3, 1) ,</v>
+        <v>max_heartrate NUMERIC(4, 1) ,</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2942,7 +2948,7 @@
         <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D26" t="str">
         <f>_xlfn.CONCAT(A26, " ", B26,  " ", C26, ",")</f>
@@ -2954,11 +2960,11 @@
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" ref="D27:D28" si="0">_xlfn.CONCAT(A27, " ", B27,  " ", C27, ",")</f>
-        <v>suffer_score INT ,</v>
+        <v>suffer_score NUMERIC(4, 1) ,</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3005,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1CCEEF-79EC-4ADE-9958-13D53D49E383}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3022,7 +3028,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3031,7 +3037,7 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -3070,7 +3076,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>123</v>
@@ -3078,20 +3084,20 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D4" s="2"/>
       <c r="F4" t="s">
         <v>128</v>
       </c>
       <c r="G4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3099,7 +3105,7 @@
         <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -3120,7 +3126,7 @@
         <v>145</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -3129,7 +3135,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>118</v>
@@ -3143,7 +3149,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
@@ -3157,7 +3163,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3165,19 +3171,19 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>119</v>
@@ -3185,13 +3191,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3199,10 +3205,10 @@
         <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>118</v>
@@ -3216,21 +3222,21 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F14" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3238,7 +3244,7 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3246,7 +3252,7 @@
         <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3254,7 +3260,7 @@
         <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3262,7 +3268,7 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3270,7 +3276,7 @@
         <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3278,7 +3284,7 @@
         <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3286,10 +3292,10 @@
         <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3297,7 +3303,7 @@
         <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3305,7 +3311,7 @@
         <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3313,7 +3319,7 @@
         <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3321,7 +3327,7 @@
         <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3329,7 +3335,7 @@
         <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3337,7 +3343,7 @@
         <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3368,10 +3374,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1">
@@ -3399,26 +3405,26 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT(A3, " ", B3, C3, ",")</f>
         <v>client_ID INT NOT NULL PRIMARY KEY,</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I3" t="str">
         <f>_xlfn.CONCAT(F3, " ", G3, H3, ",")</f>
@@ -3427,20 +3433,20 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D8" si="0">_xlfn.CONCAT(A4, " ", B4, C4, ",")</f>
         <v>client_secret NVARCHAR(64),</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I7" si="1">_xlfn.CONCAT(F4, " ", G4, H4, ",")</f>
@@ -3449,20 +3455,20 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
         <v>174</v>
-      </c>
-      <c r="B5" t="s">
-        <v>171</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>authorization_code NVARCHAR(64),</v>
       </c>
       <c r="F5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
@@ -3471,20 +3477,20 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>refresh_token NVARCHAR(64),</v>
       </c>
       <c r="F6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
@@ -3493,20 +3499,20 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>access_token NVARCHAR(64),</v>
       </c>
       <c r="F7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
@@ -3515,7 +3521,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
Minor changes to column datatypes
</commit_message>
<xml_diff>
--- a/Documentation/Strava DB data modelling.xlsx
+++ b/Documentation/Strava DB data modelling.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24202"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="629" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516B215A-1413-4844-977C-2C3DC511D897}"/>
+  <xr:revisionPtr revIDLastSave="645" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B8CD20D-DE4D-41A6-B643-943F3DD49955}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="187">
   <si>
     <t>SQL script generated via formula pt1</t>
   </si>
@@ -464,54 +464,63 @@
     <t>NOT NULL PRIMARY KEY</t>
   </si>
   <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>[name]</t>
+  </si>
+  <si>
+    <t>NUMERIC(10, 2)</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>NUMERIC(5, 1)</t>
+  </si>
+  <si>
+    <t>NOT NULL UNIQUE</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>BIT NOT NULL</t>
+  </si>
+  <si>
+    <t>NUMERIC(3, 1)</t>
+  </si>
+  <si>
+    <t>NUMERIC(4, 1)</t>
+  </si>
+  <si>
+    <t>date_amended</t>
+  </si>
+  <si>
+    <t>Reporting.FACT_activities</t>
+  </si>
+  <si>
+    <t>Reporting.DIM_activity_type</t>
+  </si>
+  <si>
+    <t>activity_type_id</t>
+  </si>
+  <si>
+    <t>staging_id</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY REFERENCES Staging.Activities(ID)</t>
+  </si>
+  <si>
     <t>NVARCHAR(50)</t>
   </si>
   <si>
-    <t>NOT NULL</t>
-  </si>
-  <si>
-    <t>NUMERIC(10, 2)</t>
-  </si>
-  <si>
-    <t>INT</t>
-  </si>
-  <si>
-    <t>NUMERIC(5, 1)</t>
-  </si>
-  <si>
-    <t>activity_type_id</t>
-  </si>
-  <si>
-    <t>NVARCHAR(100)</t>
-  </si>
-  <si>
-    <t>BIT NOT NULL</t>
-  </si>
-  <si>
-    <t>NUMERIC(3, 1)</t>
-  </si>
-  <si>
-    <t>NUMERIC(4, 1)</t>
-  </si>
-  <si>
-    <t>Reporting.FACT_activities</t>
-  </si>
-  <si>
-    <t>Reporting.DIM_activity_type</t>
-  </si>
-  <si>
-    <t>staging_id</t>
-  </si>
-  <si>
-    <t>FOREIGN KEY REFERENCES Staging.Activities(ID)</t>
-  </si>
-  <si>
     <t>Reporting.DIM_gear</t>
   </si>
   <si>
-    <t>NUMERIC(10, 1)</t>
-  </si>
-  <si>
     <t>UNIQUEIDENTIFER</t>
   </si>
   <si>
@@ -524,19 +533,19 @@
     <t>Staging - DIM_date</t>
   </si>
   <si>
+    <t>FK?</t>
+  </si>
+  <si>
+    <t>date_id</t>
+  </si>
+  <si>
+    <t>start_date_id</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY REFERENCES Reporting.DIM_date(date_id)</t>
+  </si>
+  <si>
     <t>FK</t>
-  </si>
-  <si>
-    <t>date_id</t>
-  </si>
-  <si>
-    <t>start_date_id</t>
-  </si>
-  <si>
-    <t>FOREIGN KEY REFERENCES Reporting.DIM_date(date_id)</t>
-  </si>
-  <si>
-    <t>NUMERIC(2, 2)</t>
   </si>
   <si>
     <t>Config.API_credentials</t>
@@ -1882,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BDDA7B-2722-47CB-9F85-BD1E88FF284B}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2615,8 +2624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77B814F-9F70-4B91-9F92-4045C1E00E64}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2679,12 +2688,12 @@
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(A4, " ", B4,  " ", C4, ",")</f>
-        <v>athlete_id NVARCHAR(50) NOT NULL,</v>
+        <v>athlete_id VARCHAR(50) NOT NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
         <v>125</v>
@@ -2694,7 +2703,7 @@
       </c>
       <c r="D5" t="str">
         <f>_xlfn.CONCAT(A5, " ", B5,  " ", C5, ",")</f>
-        <v>name NVARCHAR(250) NOT NULL,</v>
+        <v>[name] NVARCHAR(250) NOT NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2702,7 +2711,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D6" t="str">
         <f>_xlfn.CONCAT(A6, " ", B6,  " ", C6, ",")</f>
@@ -2714,7 +2723,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D7" t="str">
         <f>_xlfn.CONCAT(A7, " ", B7,  " ", C7, ",")</f>
@@ -2726,7 +2735,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D8" t="str">
         <f>_xlfn.CONCAT(A8, " ", B8,  " ", C8, ",")</f>
@@ -2738,7 +2747,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D9" t="str">
         <f>_xlfn.CONCAT(A9, " ", B9,  " ", C9, ",")</f>
@@ -2747,14 +2756,14 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D10" t="str">
         <f>_xlfn.CONCAT(A10, " ", B10,  " ", C10, ",")</f>
-        <v>activity_type_id INT ,</v>
+        <v>activity_type INT ,</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2762,11 +2771,11 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D11" t="str">
         <f>_xlfn.CONCAT(A11, " ", B11,  " ", C11, ",")</f>
-        <v>workout_type INT ,</v>
+        <v>workout_type VARCHAR(50) ,</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2777,11 +2786,11 @@
         <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D12" t="str">
         <f>_xlfn.CONCAT(A12, " ", B12,  " ", C12, ",")</f>
-        <v>activity_id NVARCHAR(50) NOT NULL,</v>
+        <v>activity_id VARCHAR(50) NOT NULL UNIQUE,</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2789,11 +2798,11 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.CONCAT(A13, " ", B13,  " ", C13, ",")</f>
-        <v>external_id NVARCHAR(100) ,</v>
+        <v>external_id VARCHAR(100) ,</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2816,7 +2825,7 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D15" t="str">
         <f>_xlfn.CONCAT(A15, " ", B15,  " ", C15, ",")</f>
@@ -2828,7 +2837,7 @@
         <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D16" t="str">
         <f>_xlfn.CONCAT(A16, " ", B16,  " ", C16, ",")</f>
@@ -2840,7 +2849,7 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D17" t="str">
         <f>_xlfn.CONCAT(A17, " ", B17,  " ", C17, ",")</f>
@@ -2852,7 +2861,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D18" t="str">
         <f>_xlfn.CONCAT(A18, " ", B18,  " ", C18, ",")</f>
@@ -2864,7 +2873,7 @@
         <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D19" t="str">
         <f>_xlfn.CONCAT(A19, " ", B19,  " ", C19, ",")</f>
@@ -2876,7 +2885,7 @@
         <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D20" t="str">
         <f>_xlfn.CONCAT(A20, " ", B20,  " ", C20, ",")</f>
@@ -2892,7 +2901,7 @@
       </c>
       <c r="D21" t="str">
         <f>_xlfn.CONCAT(A21, " ", B21,  " ", C21, ",")</f>
-        <v>gear_id NVARCHAR(50) ,</v>
+        <v>gear_id VARCHAR(50) ,</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2900,7 +2909,7 @@
         <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D22" t="str">
         <f>_xlfn.CONCAT(A22, " ", B22,  " ", C22, ",")</f>
@@ -2912,7 +2921,7 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D23" t="str">
         <f>_xlfn.CONCAT(A23, " ", B23,  " ", C23, ",")</f>
@@ -2924,7 +2933,7 @@
         <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D24" t="str">
         <f>_xlfn.CONCAT(A24, " ", B24,  " ", C24, ",")</f>
@@ -2936,7 +2945,7 @@
         <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D25" t="str">
         <f>_xlfn.CONCAT(A25, " ", B25,  " ", C25, ",")</f>
@@ -2948,7 +2957,7 @@
         <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D26" t="str">
         <f>_xlfn.CONCAT(A26, " ", B26,  " ", C26, ",")</f>
@@ -2960,7 +2969,7 @@
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" ref="D27:D28" si="0">_xlfn.CONCAT(A27, " ", B27,  " ", C27, ",")</f>
@@ -2984,7 +2993,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>135</v>
@@ -2994,7 +3003,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" ref="D28:D29" si="1">_xlfn.CONCAT(A29, " ", B29,  " ", C29)</f>
-        <v>date_processed DATETIME DEFAULT GETDATE()</v>
+        <v>date_amended DATETIME DEFAULT GETDATE()</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3011,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1CCEEF-79EC-4ADE-9958-13D53D49E383}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3028,7 +3037,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3037,7 +3046,7 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -3076,7 +3085,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>123</v>
@@ -3084,20 +3093,20 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D4" s="2"/>
       <c r="F4" t="s">
         <v>128</v>
       </c>
       <c r="G4" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3105,14 +3114,14 @@
         <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
       </c>
       <c r="D5" t="str">
         <f>_xlfn.CONCAT(A5, " ", B5,  " ", C5, ",")</f>
-        <v>athlete_id INT NOT NULL,</v>
+        <v>athlete_id VARCHAR(50) NOT NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3126,7 +3135,7 @@
         <v>145</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -3135,7 +3144,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>118</v>
@@ -3149,7 +3158,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
@@ -3163,7 +3172,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3171,19 +3180,19 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>119</v>
@@ -3191,13 +3200,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3205,10 +3214,10 @@
         <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>118</v>
@@ -3222,21 +3231,21 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3244,7 +3253,7 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3252,7 +3261,7 @@
         <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3260,7 +3269,7 @@
         <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3268,7 +3277,7 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3276,7 +3285,7 @@
         <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3284,7 +3293,7 @@
         <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3295,7 +3304,7 @@
         <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3303,7 +3312,7 @@
         <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3311,7 +3320,7 @@
         <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3319,7 +3328,7 @@
         <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3327,7 +3336,7 @@
         <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3335,7 +3344,7 @@
         <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3343,7 +3352,7 @@
         <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3374,10 +3383,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1">
@@ -3405,26 +3414,26 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT(A3, " ", B3, C3, ",")</f>
         <v>client_ID INT NOT NULL PRIMARY KEY,</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I3" t="str">
         <f>_xlfn.CONCAT(F3, " ", G3, H3, ",")</f>
@@ -3433,20 +3442,20 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D8" si="0">_xlfn.CONCAT(A4, " ", B4, C4, ",")</f>
         <v>client_secret NVARCHAR(64),</v>
       </c>
       <c r="F4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I7" si="1">_xlfn.CONCAT(F4, " ", G4, H4, ",")</f>
@@ -3455,20 +3464,20 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" t="s">
         <v>177</v>
-      </c>
-      <c r="B5" t="s">
-        <v>174</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>authorization_code NVARCHAR(64),</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
@@ -3477,20 +3486,20 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>refresh_token NVARCHAR(64),</v>
       </c>
       <c r="F6" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
@@ -3499,20 +3508,20 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>access_token NVARCHAR(64),</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
@@ -3521,7 +3530,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B8" t="s">
         <v>135</v>

</xml_diff>